<commit_message>
waiting to upload the WGBS to SRA
</commit_message>
<xml_diff>
--- a/data/SRA_metadata_acc.xlsx
+++ b/data/SRA_metadata_acc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="2500" windowWidth="29180" windowHeight="21520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9800" yWindow="2200" windowWidth="42640" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Info and Instructions" sheetId="3" r:id="rId1"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="303">
   <si>
     <t>filename</t>
   </si>
@@ -1182,6 +1182,135 @@
   </si>
   <si>
     <t>WGBS of 20 teosintes</t>
+  </si>
+  <si>
+    <t>paired</t>
+  </si>
+  <si>
+    <t>fastq</t>
+  </si>
+  <si>
+    <t>We conducted whole genome sequencing (WGS) and whole genome biosulfite sequencing (WGBS) on 20 teosinte lineswith the average coverages of about 30× and 5×, respectively</t>
+  </si>
+  <si>
+    <t>JRA1_CTTGTA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRA1_CTTGTA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB1_NoIndex_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB1_NoIndex_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC1_AGTTCC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC1_AGTTCC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD1_ATGTCA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD1_ATGTCA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRE1_CCGTCC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRE1_CCGTCC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRF1_NoIndex_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRF1_NoIndex_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRG1_GTGAAA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRG1_GTGAAA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRH1_CGATGT_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRH1_CGATGT_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRA2_TGACCA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRA2_TGACCA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB2_NoIndex_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB2_NoIndex_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC2_GCCAAT_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC2_GCCAAT_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD2_CAGATC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD2_CAGATC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRE2_CTTGTA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRE2_CTTGTA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRF2_AGTCAA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRF2_AGTCAA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRG2_AGTTCC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRG2_AGTTCC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRH2_ATGTCA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRH2_ATGTCA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRA3_CCGTCC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRA3_CCGTCC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB3_GTCCGC_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRB3_GTCCGC_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC3_GTGAAA_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRC3_GTGAAA_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD3_NoIndex_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>JRD3_NoIndex_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -2198,7 +2327,7 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2481,7 +2610,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2569,13 +2698,36 @@
       <c r="D2" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M2" t="s">
+        <v>263</v>
+      </c>
+      <c r="N2" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
@@ -2590,13 +2742,36 @@
       <c r="D3" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="E3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M3" t="s">
+        <v>265</v>
+      </c>
+      <c r="N3" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
@@ -2611,13 +2786,36 @@
       <c r="D4" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M4" t="s">
+        <v>267</v>
+      </c>
+      <c r="N4" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
@@ -2632,13 +2830,36 @@
       <c r="D5" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M5" t="s">
+        <v>269</v>
+      </c>
+      <c r="N5" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="55" t="s">
@@ -2653,13 +2874,36 @@
       <c r="D6" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M6" t="s">
+        <v>271</v>
+      </c>
+      <c r="N6" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
@@ -2674,13 +2918,36 @@
       <c r="D7" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="E7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M7" t="s">
+        <v>273</v>
+      </c>
+      <c r="N7" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="s">
@@ -2695,13 +2962,36 @@
       <c r="D8" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="E8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M8" t="s">
+        <v>275</v>
+      </c>
+      <c r="N8" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
@@ -2716,13 +3006,36 @@
       <c r="D9" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M9" t="s">
+        <v>277</v>
+      </c>
+      <c r="N9" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="s">
@@ -2737,13 +3050,36 @@
       <c r="D10" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M10" t="s">
+        <v>279</v>
+      </c>
+      <c r="N10" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
@@ -2758,13 +3094,36 @@
       <c r="D11" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N11" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
@@ -2779,13 +3138,36 @@
       <c r="D12" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="L12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M12" t="s">
+        <v>283</v>
+      </c>
+      <c r="N12" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
@@ -2800,13 +3182,36 @@
       <c r="D13" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="L13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M13" t="s">
+        <v>285</v>
+      </c>
+      <c r="N13" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="s">
@@ -2821,13 +3226,36 @@
       <c r="D14" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="L14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M14" t="s">
+        <v>287</v>
+      </c>
+      <c r="N14" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="s">
@@ -2842,13 +3270,36 @@
       <c r="D15" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="L15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M15" t="s">
+        <v>289</v>
+      </c>
+      <c r="N15" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
@@ -2863,15 +3314,38 @@
       <c r="D16" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M16" t="s">
+        <v>291</v>
+      </c>
+      <c r="N16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
         <v>218</v>
       </c>
@@ -2884,15 +3358,38 @@
       <c r="D17" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E17" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M17" t="s">
+        <v>293</v>
+      </c>
+      <c r="N17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="55" t="s">
         <v>218</v>
       </c>
@@ -2905,15 +3402,38 @@
       <c r="D18" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M18" t="s">
+        <v>295</v>
+      </c>
+      <c r="N18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
         <v>218</v>
       </c>
@@ -2926,15 +3446,38 @@
       <c r="D19" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="L19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M19" t="s">
+        <v>297</v>
+      </c>
+      <c r="N19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
         <v>218</v>
       </c>
@@ -2947,15 +3490,38 @@
       <c r="D20" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="L20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+      <c r="E20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M20" t="s">
+        <v>299</v>
+      </c>
+      <c r="N20" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
         <v>218</v>
       </c>
@@ -2968,15 +3534,38 @@
       <c r="D21" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="M21" t="s">
+        <v>301</v>
+      </c>
+      <c r="N21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -2985,7 +3574,7 @@
       <c r="J22" s="15"/>
       <c r="L22" s="15"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2994,7 +3583,7 @@
       <c r="J23" s="15"/>
       <c r="L23" s="15"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -3003,7 +3592,7 @@
       <c r="J24" s="15"/>
       <c r="L24" s="15"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -3012,7 +3601,7 @@
       <c r="J25" s="15"/>
       <c r="L25" s="15"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -3021,7 +3610,7 @@
       <c r="J26" s="15"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -3030,7 +3619,7 @@
       <c r="J27" s="15"/>
       <c r="L27" s="15"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -3039,7 +3628,7 @@
       <c r="J28" s="15"/>
       <c r="L28" s="15"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -3048,7 +3637,7 @@
       <c r="J29" s="15"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -3057,7 +3646,7 @@
       <c r="J30" s="15"/>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -3066,7 +3655,7 @@
       <c r="J31" s="15"/>
       <c r="L31" s="15"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>

</xml_diff>